<commit_message>
feat: add exhibition images page
</commit_message>
<xml_diff>
--- a/seeders/seedsRawData.xlsx
+++ b/seeders/seedsRawData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smili\nodeJs\art_collection\seeders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AE2C9F-9BBF-4D11-BC08-BD5F07C4A76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02411324-6828-421F-A910-F586D18607E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{D8701844-A823-4B3C-B3BD-3BDA1D25A239}"/>
+    <workbookView xWindow="59340" yWindow="0" windowWidth="14460" windowHeight="17400" activeTab="7" xr2:uid="{D8701844-A823-4B3C-B3BD-3BDA1D25A239}"/>
   </bookViews>
   <sheets>
     <sheet name="artist" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1920" uniqueCount="908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2001" uniqueCount="932">
   <si>
     <t>name</t>
   </si>
@@ -2951,6 +2951,78 @@
   </si>
   <si>
     <t>待確認是否有圖可取得，不然就不放這些作品、exhibitionArtwork也刪掉</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/WxXYeI3.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/zsKyza6.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/bZYBMHB.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/414VqdZ.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/HCbfLU8.jpg</t>
+  </si>
+  <si>
+    <t>artist</t>
+  </si>
+  <si>
+    <t>space</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/udcMzmg.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/NwhA4hV.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/1hQWekk.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/CqUpDYj.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/4Kh679O.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/StrxRp8.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/edfvZIu.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/vI5hrn4.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/O10lhkD.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/8I3fJb1.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/vy0BJFZ.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/LVyK5EY.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/MqS6zl7.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Xo5Fswo.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/NnKowVh.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/jKzwLdU.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/GBGtUeM.jpg</t>
   </si>
 </sst>
 </file>
@@ -5410,7 +5482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9B7D3C-9641-4757-A4D3-84371419D231}">
   <dimension ref="A1:M178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A153" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H178" sqref="H178"/>
     </sheetView>
   </sheetViews>
@@ -9381,7 +9453,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="43">
+    <row r="107" spans="1:13" ht="28.7">
       <c r="A107" s="21" t="s">
         <v>420</v>
       </c>
@@ -12353,7 +12425,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15.7">
+    <row r="12" spans="1:15" ht="31.35">
       <c r="A12" s="12" t="s">
         <v>151</v>
       </c>
@@ -14199,10 +14271,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D559C658-0E26-48C2-9425-97D0AB2EAD7F}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
@@ -14260,43 +14332,340 @@
         <v>71</v>
       </c>
       <c r="B5" t="s">
+        <v>911</v>
+      </c>
+      <c r="C5" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.35">
+      <c r="A6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
+        <v>923</v>
+      </c>
+      <c r="C6" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.35">
+      <c r="A7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" t="s">
+        <v>924</v>
+      </c>
+      <c r="C7" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.35">
+      <c r="A8" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" t="s">
         <v>697</v>
-      </c>
-      <c r="C5" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="8" t="s">
-        <v>704</v>
-      </c>
-      <c r="B6" t="s">
-        <v>700</v>
-      </c>
-      <c r="C6" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="8" t="s">
-        <v>704</v>
-      </c>
-      <c r="B7" t="s">
-        <v>701</v>
-      </c>
-      <c r="C7" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.35">
-      <c r="A8" s="44" t="s">
-        <v>703</v>
-      </c>
-      <c r="B8" t="s">
-        <v>702</v>
       </c>
       <c r="C8" t="s">
         <v>698</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.35">
+      <c r="A9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" t="s">
+        <v>925</v>
+      </c>
+      <c r="C9" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.35">
+      <c r="A10" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>926</v>
+      </c>
+      <c r="C10" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.35">
+      <c r="A11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>927</v>
+      </c>
+      <c r="C11" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.35">
+      <c r="A12" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
+        <v>928</v>
+      </c>
+      <c r="C12" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.35">
+      <c r="A13" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
+        <v>929</v>
+      </c>
+      <c r="C13" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.35">
+      <c r="A14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
+        <v>930</v>
+      </c>
+      <c r="C14" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.35">
+      <c r="A15" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>931</v>
+      </c>
+      <c r="C15" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.35">
+      <c r="A16" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" t="s">
+        <v>910</v>
+      </c>
+      <c r="C16" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="B17" t="s">
+        <v>700</v>
+      </c>
+      <c r="C17" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="B18" t="s">
+        <v>701</v>
+      </c>
+      <c r="C18" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="B19" t="s">
+        <v>908</v>
+      </c>
+      <c r="C19" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="B20" t="s">
+        <v>909</v>
+      </c>
+      <c r="C20" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="B21" t="s">
+        <v>910</v>
+      </c>
+      <c r="C21" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="B22" t="s">
+        <v>911</v>
+      </c>
+      <c r="C22" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="B23" t="s">
+        <v>912</v>
+      </c>
+      <c r="C23" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="B24" t="s">
+        <v>915</v>
+      </c>
+      <c r="C24" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="B25" t="s">
+        <v>916</v>
+      </c>
+      <c r="C25" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="8" t="s">
+        <v>704</v>
+      </c>
+      <c r="B26" t="s">
+        <v>917</v>
+      </c>
+      <c r="C26" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.35">
+      <c r="A27" s="44" t="s">
+        <v>703</v>
+      </c>
+      <c r="B27" t="s">
+        <v>702</v>
+      </c>
+      <c r="C27" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.35">
+      <c r="A28" s="44" t="s">
+        <v>703</v>
+      </c>
+      <c r="B28" t="s">
+        <v>911</v>
+      </c>
+      <c r="C28" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.35">
+      <c r="A29" s="44" t="s">
+        <v>703</v>
+      </c>
+      <c r="B29" t="s">
+        <v>917</v>
+      </c>
+      <c r="C29" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.35">
+      <c r="A30" s="44" t="s">
+        <v>703</v>
+      </c>
+      <c r="B30" t="s">
+        <v>918</v>
+      </c>
+      <c r="C30" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.35">
+      <c r="A31" s="44" t="s">
+        <v>703</v>
+      </c>
+      <c r="B31" t="s">
+        <v>919</v>
+      </c>
+      <c r="C31" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.35">
+      <c r="A32" s="44" t="s">
+        <v>703</v>
+      </c>
+      <c r="B32" t="s">
+        <v>920</v>
+      </c>
+      <c r="C32" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.35">
+      <c r="A33" s="44" t="s">
+        <v>703</v>
+      </c>
+      <c r="B33" t="s">
+        <v>921</v>
+      </c>
+      <c r="C33" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.35">
+      <c r="A34" s="44" t="s">
+        <v>703</v>
+      </c>
+      <c r="B34" t="s">
+        <v>922</v>
+      </c>
+      <c r="C34" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.35">
+      <c r="A35" s="44" t="s">
+        <v>703</v>
+      </c>
+      <c r="B35" t="s">
+        <v>923</v>
+      </c>
+      <c r="C35" t="s">
+        <v>914</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add url_origin column to artwork images and seed data
</commit_message>
<xml_diff>
--- a/seeders/seedsRawData.xlsx
+++ b/seeders/seedsRawData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smili\nodeJs\art_collection\seeders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E924310-267C-41DE-9257-C0AE7AFDE532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC8D9E6-A3CB-4398-AE87-14E6DC102EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45000" yWindow="0" windowWidth="14400" windowHeight="17400" activeTab="2" xr2:uid="{D8701844-A823-4B3C-B3BD-3BDA1D25A239}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12920" activeTab="2" xr2:uid="{D8701844-A823-4B3C-B3BD-3BDA1D25A239}"/>
   </bookViews>
   <sheets>
     <sheet name="artist" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2000" uniqueCount="932">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="1094">
   <si>
     <t>name</t>
   </si>
@@ -3020,6 +3020,492 @@
   </si>
   <si>
     <t>29.3x14.6x18.4</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/4dkTPhzm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/0qO8s3Xm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/c1G8kJYm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/QQVulRIm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/JtBAojtm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/VnoxP59m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/MSntSExm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/kAj8WXIm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/JLyfezmm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/xvYXzWSm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/QOYwDemm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/fDlleKwm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/09qcIExm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/qRdhzDWm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/f3gO20Sm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/3LxQrjlm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/9w8HsWIm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/lJU7Xk8m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/G4exzbqm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/fw85ACgm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/LGlBcKRm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Je0LoyCm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Z10VyRFm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Ce3OzzVm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/JA0renbm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/x7JTYEYm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/vDmeZK1m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/yAfmpmKm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/1SuDiqom.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/aAoyC2Tm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/JhAB3uVm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/FjkJ7tKm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/ZR8pdMkm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/lob19iom.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/xlopoS9m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/6nnn8P7m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/lAvacI6m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/0Cf1Y1Lm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/0KvlcoMm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/0rCdU0mm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/0vHcKJrm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/0y1OV1hm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/395riYSm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/3FlSnepm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/62zOFYum.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/8RVrZrTm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/9ERXAz8m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/9nBGTsBm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/9QhMGvhm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Agb9Z5Wm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/DAcgu2Fm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/DrUa3nWm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/E1b5zSym.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Enf2Y6Rm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/EQ3tyiXm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/EZ8gUO1m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/FIvXzYKm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/G1oR3bEm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/GsDO5ezm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/HolsUtNm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/IvU8aa5m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/IZjAD2jm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/jEE4tewm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/KvkPrcFm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/kvR3Dd4m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/M2mY4Lxm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/N9TLzEDm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/nURTPOzm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/OsrUz0Sm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/oWCWAUUm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/PckYviom.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/PFoq00Fm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/phFUHVcm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/pJUaWI2m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Q3YVr1mm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/QyEWYxsm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/r1XbwxOm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/rmNzjF7m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/RU4wdxLm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/ruS9nfNm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/s5XkYcHm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/scjC2yHm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/SDDLbfam.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/SNagijYm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/stOHELem.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/t170xN6m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/tR8wNmdm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/U4wtUspm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/v1yNjcUm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/V5l6N0Fm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/VdbxZvjm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Vn3YwX7m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/WIFtsCYm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/WLt1sbVm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/WUj0NYhm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/xAybNnxm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/XLeOcssm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/XqFksmem.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/xqnSk5vm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/yZwWaGum.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/zNrobM6m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/oFauDDpm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Qi9mHzKm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Ih9ggS6m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/xUNy89gm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/mQLoKdJm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/dZMQJtHm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/H74HIfdm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/qnYMz7tm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/KUqMOkSm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/H8Mt16cm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/lwIV92gm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/lDYA1Bwm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/8ZFxamVm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/zP9GmCDm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/DvLgNmKm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/aTlOtLam.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Z73kPFfm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/0UmbJEFm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/uZ4bgSCm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/HdixVHXm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/iZUeN7om.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/oUvmijrm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/NdB8VzQm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/HI0YLJam.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/tqOedAYm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/e1pdJkAm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/QQyfDjSm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/po1WEgim.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/ruWY0gBm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/hOaZRbbm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/iQN8Yunm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/6aWRb3Im.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/zmuLD8tm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/sajim6Nm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/36NOAwum.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Ir9GZXym.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/ls6vjvHm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/TnYZEyCm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/uFd4XkNm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/W3AoXCem.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/GMPpX5dm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/ERLmr3um.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/yLXKRTsm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/FS62vvYm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/IkZbkZGm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/1ZWNpL8m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/rRIPeOdm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/U3Sl0eHm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/EfgzuNHm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/pzA4y0cm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/vV982Z4m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/kiaOduom.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/ZrEqyuDm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/ST20xqom.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/NhrZn0gm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/QlOEwgMm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/aBl5bEjm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/GjASiq0m.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Df4o7lzm.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/CKjXZrjm.jpg</t>
+  </si>
+  <si>
+    <t>url_origin</t>
   </si>
 </sst>
 </file>
@@ -3234,7 +3720,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3367,16 +3853,10 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -3400,6 +3880,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -5255,131 +5736,127 @@
     </row>
     <row r="15" spans="1:4" ht="15.7">
       <c r="A15" s="1"/>
-      <c r="C15" s="46"/>
+      <c r="C15" s="45"/>
     </row>
     <row r="16" spans="1:4" ht="15.7">
       <c r="A16" s="2"/>
-      <c r="C16" s="45"/>
     </row>
     <row r="17" spans="1:3" ht="15.7">
       <c r="A17" s="2"/>
-      <c r="C17" s="45"/>
     </row>
     <row r="18" spans="1:3" ht="15.7">
       <c r="A18" s="2"/>
-      <c r="C18" s="49"/>
+      <c r="C18" s="47"/>
     </row>
     <row r="19" spans="1:3" ht="15.7">
       <c r="A19" s="2"/>
-      <c r="C19" s="47"/>
+      <c r="C19" s="45"/>
     </row>
     <row r="20" spans="1:3" ht="15.7">
       <c r="A20" s="2"/>
-      <c r="C20" s="48"/>
+      <c r="C20" s="46"/>
     </row>
     <row r="21" spans="1:3" ht="15.7">
       <c r="A21" s="2"/>
-      <c r="C21" s="48"/>
+      <c r="C21" s="46"/>
     </row>
     <row r="22" spans="1:3" ht="15.7">
       <c r="A22" s="2"/>
-      <c r="C22" s="48"/>
+      <c r="C22" s="46"/>
     </row>
     <row r="23" spans="1:3" ht="15.7">
       <c r="A23" s="2"/>
-      <c r="C23" s="48"/>
+      <c r="C23" s="46"/>
     </row>
     <row r="24" spans="1:3" ht="15.7">
       <c r="A24" s="2"/>
-      <c r="C24" s="48"/>
+      <c r="C24" s="46"/>
     </row>
     <row r="25" spans="1:3" ht="15.7">
       <c r="A25" s="2"/>
-      <c r="C25" s="45"/>
     </row>
     <row r="26" spans="1:3" ht="15.7">
       <c r="A26" s="2"/>
-      <c r="C26" s="48"/>
+      <c r="C26" s="46"/>
     </row>
     <row r="27" spans="1:3" ht="15.7">
       <c r="A27" s="2"/>
-      <c r="C27" s="48"/>
+      <c r="C27" s="46"/>
     </row>
     <row r="28" spans="1:3" ht="15.7">
       <c r="A28" s="2"/>
-      <c r="C28" s="48"/>
+      <c r="C28" s="46"/>
     </row>
     <row r="29" spans="1:3" ht="15.7">
       <c r="A29" s="2"/>
-      <c r="C29" s="48"/>
+      <c r="C29" s="46"/>
     </row>
     <row r="30" spans="1:3" ht="15.7">
       <c r="A30" s="2"/>
-      <c r="C30" s="48"/>
+      <c r="C30" s="46"/>
     </row>
     <row r="31" spans="1:3" ht="15.7">
       <c r="A31" s="2"/>
-      <c r="C31" s="48"/>
+      <c r="C31" s="46"/>
     </row>
     <row r="32" spans="1:3" ht="15.7">
       <c r="A32" s="2"/>
-      <c r="C32" s="48"/>
+      <c r="C32" s="46"/>
     </row>
     <row r="33" spans="1:3" ht="15.7">
       <c r="A33" s="2"/>
-      <c r="C33" s="46"/>
+      <c r="C33" s="45"/>
     </row>
     <row r="34" spans="1:3" ht="15.7">
       <c r="A34" s="2"/>
-      <c r="C34" s="48"/>
+      <c r="C34" s="46"/>
     </row>
     <row r="35" spans="1:3" ht="15.7">
       <c r="A35" s="2"/>
-      <c r="C35" s="46"/>
+      <c r="C35" s="45"/>
     </row>
     <row r="36" spans="1:3" ht="15.7">
       <c r="A36" s="3"/>
-      <c r="C36" s="48"/>
+      <c r="C36" s="46"/>
     </row>
     <row r="37" spans="1:3" ht="15.7">
       <c r="A37" s="4"/>
-      <c r="C37" s="45"/>
     </row>
     <row r="38" spans="1:3" ht="15.7">
       <c r="A38" s="4"/>
-      <c r="C38" s="48"/>
+      <c r="C38" s="46"/>
     </row>
     <row r="39" spans="1:3" ht="15.7">
       <c r="A39" s="4"/>
-      <c r="C39" s="46"/>
+      <c r="C39" s="45"/>
     </row>
     <row r="40" spans="1:3" ht="15.7">
       <c r="A40" s="4"/>
-      <c r="C40" s="48"/>
+      <c r="C40" s="46"/>
     </row>
     <row r="41" spans="1:3" ht="15.7">
       <c r="A41" s="4"/>
-      <c r="C41" s="48"/>
+      <c r="C41" s="46"/>
     </row>
     <row r="42" spans="1:3" ht="15.7">
       <c r="A42" s="4"/>
-      <c r="C42" s="48"/>
+      <c r="C42" s="46"/>
     </row>
     <row r="43" spans="1:3" ht="15.7">
       <c r="A43" s="4"/>
-      <c r="C43" s="48"/>
+      <c r="C43" s="46"/>
     </row>
     <row r="44" spans="1:3" ht="15.7">
       <c r="A44" s="1"/>
-      <c r="C44" s="48"/>
+      <c r="C44" s="46"/>
     </row>
     <row r="45" spans="1:3" ht="15.7">
       <c r="A45" s="1"/>
-      <c r="C45" s="48"/>
+      <c r="C45" s="46"/>
     </row>
     <row r="46" spans="1:3" ht="15.7">
       <c r="A46" s="5"/>
-      <c r="C46" s="48"/>
+      <c r="C46" s="46"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5489,10 +5966,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9B7D3C-9641-4757-A4D3-84371419D231}">
-  <dimension ref="A1:M178"/>
+  <dimension ref="A1:N178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L156" sqref="L156"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35"/>
@@ -5505,9 +5982,10 @@
     <col min="7" max="7" width="13.41015625" customWidth="1"/>
     <col min="8" max="11" width="8.9375" customWidth="1"/>
     <col min="12" max="12" width="35.703125" customWidth="1"/>
+    <col min="13" max="13" width="37.234375" style="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>205</v>
       </c>
@@ -5542,13 +6020,16 @@
         <v>615</v>
       </c>
       <c r="L1" t="s">
+        <v>1093</v>
+      </c>
+      <c r="M1" t="s">
         <v>689</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.7">
+    <row r="2" spans="1:14" ht="15.7">
       <c r="A2" s="12" t="s">
         <v>77</v>
       </c>
@@ -5581,11 +6062,14 @@
       <c r="L2" t="s">
         <v>805</v>
       </c>
-      <c r="M2" s="40" t="s">
+      <c r="M2" s="53" t="s">
+        <v>932</v>
+      </c>
+      <c r="N2" s="40" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.7">
+    <row r="3" spans="1:14" ht="15.7">
       <c r="A3" s="12" t="s">
         <v>80</v>
       </c>
@@ -5620,11 +6104,14 @@
       <c r="L3" t="s">
         <v>806</v>
       </c>
-      <c r="M3" s="40" t="s">
+      <c r="M3" s="53" t="s">
+        <v>933</v>
+      </c>
+      <c r="N3" s="40" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.7">
+    <row r="4" spans="1:14" ht="15.7">
       <c r="A4" s="12" t="s">
         <v>84</v>
       </c>
@@ -5657,11 +6144,14 @@
       <c r="L4" t="s">
         <v>807</v>
       </c>
-      <c r="M4" s="40" t="s">
+      <c r="M4" s="53" t="s">
+        <v>934</v>
+      </c>
+      <c r="N4" s="40" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.7">
+    <row r="5" spans="1:14" ht="15.7">
       <c r="A5" s="15" t="s">
         <v>86</v>
       </c>
@@ -5694,11 +6184,14 @@
       <c r="L5" t="s">
         <v>808</v>
       </c>
-      <c r="M5" s="40" t="s">
+      <c r="M5" s="53" t="s">
+        <v>935</v>
+      </c>
+      <c r="N5" s="40" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="15.7">
+    <row r="6" spans="1:14" ht="15.7">
       <c r="A6" s="15" t="s">
         <v>89</v>
       </c>
@@ -5731,11 +6224,14 @@
       <c r="L6" t="s">
         <v>810</v>
       </c>
-      <c r="M6" s="40" t="s">
+      <c r="M6" s="53" t="s">
+        <v>936</v>
+      </c>
+      <c r="N6" s="40" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="15.7">
+    <row r="7" spans="1:14" ht="15.7">
       <c r="A7" s="12" t="s">
         <v>92</v>
       </c>
@@ -5768,11 +6264,14 @@
       <c r="L7" t="s">
         <v>811</v>
       </c>
-      <c r="M7" s="40" t="s">
+      <c r="M7" s="53" t="s">
+        <v>937</v>
+      </c>
+      <c r="N7" s="40" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="15.7">
+    <row r="8" spans="1:14" ht="15.7">
       <c r="A8" s="12" t="s">
         <v>95</v>
       </c>
@@ -5805,11 +6304,14 @@
       <c r="L8" t="s">
         <v>812</v>
       </c>
-      <c r="M8" s="40" t="s">
+      <c r="M8" s="53" t="s">
+        <v>938</v>
+      </c>
+      <c r="N8" s="40" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.7">
+    <row r="9" spans="1:14" ht="15.7">
       <c r="A9" s="12" t="s">
         <v>98</v>
       </c>
@@ -5842,11 +6344,14 @@
       <c r="L9" t="s">
         <v>816</v>
       </c>
-      <c r="M9" s="40" t="s">
+      <c r="M9" s="53" t="s">
+        <v>939</v>
+      </c>
+      <c r="N9" s="40" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="15.7">
+    <row r="10" spans="1:14" ht="15.7">
       <c r="A10" s="12" t="s">
         <v>104</v>
       </c>
@@ -5879,11 +6384,14 @@
       <c r="L10" t="s">
         <v>817</v>
       </c>
-      <c r="M10" s="40" t="s">
+      <c r="M10" s="53" t="s">
+        <v>940</v>
+      </c>
+      <c r="N10" s="40" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="15.7">
+    <row r="11" spans="1:14" ht="15.7">
       <c r="A11" s="12" t="s">
         <v>107</v>
       </c>
@@ -5916,11 +6424,14 @@
       <c r="L11" t="s">
         <v>818</v>
       </c>
-      <c r="M11" s="40" t="s">
+      <c r="M11" s="53" t="s">
+        <v>941</v>
+      </c>
+      <c r="N11" s="40" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="15.7">
+    <row r="12" spans="1:14" ht="15.7">
       <c r="A12" s="12" t="s">
         <v>111</v>
       </c>
@@ -5953,11 +6464,14 @@
       <c r="L12" t="s">
         <v>819</v>
       </c>
-      <c r="M12" s="40" t="s">
+      <c r="M12" s="53" t="s">
+        <v>942</v>
+      </c>
+      <c r="N12" s="40" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="15.7">
+    <row r="13" spans="1:14" ht="15.7">
       <c r="A13" s="12" t="s">
         <v>114</v>
       </c>
@@ -5990,11 +6504,14 @@
       <c r="L13" t="s">
         <v>820</v>
       </c>
-      <c r="M13" s="40" t="s">
+      <c r="M13" s="53" t="s">
+        <v>943</v>
+      </c>
+      <c r="N13" s="40" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.7">
+    <row r="14" spans="1:14" ht="15.7">
       <c r="A14" s="15" t="s">
         <v>117</v>
       </c>
@@ -6029,11 +6546,14 @@
       <c r="L14" t="s">
         <v>821</v>
       </c>
-      <c r="M14" s="40" t="s">
+      <c r="M14" s="53" t="s">
+        <v>944</v>
+      </c>
+      <c r="N14" s="40" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="15.7">
+    <row r="15" spans="1:14" ht="15.7">
       <c r="A15" s="12" t="s">
         <v>120</v>
       </c>
@@ -6068,11 +6588,14 @@
       <c r="L15" t="s">
         <v>822</v>
       </c>
-      <c r="M15" s="40" t="s">
+      <c r="M15" s="53" t="s">
+        <v>945</v>
+      </c>
+      <c r="N15" s="40" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.7">
+    <row r="16" spans="1:14" ht="15.7">
       <c r="A16" s="12" t="s">
         <v>123</v>
       </c>
@@ -6107,11 +6630,14 @@
       <c r="L16" t="s">
         <v>823</v>
       </c>
-      <c r="M16" s="40" t="s">
+      <c r="M16" s="53" t="s">
+        <v>946</v>
+      </c>
+      <c r="N16" s="40" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.7">
+    <row r="17" spans="1:14" ht="15.7">
       <c r="A17" s="12" t="s">
         <v>126</v>
       </c>
@@ -6146,11 +6672,14 @@
       <c r="L17" t="s">
         <v>824</v>
       </c>
-      <c r="M17" s="40" t="s">
+      <c r="M17" s="53" t="s">
+        <v>947</v>
+      </c>
+      <c r="N17" s="40" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.7">
+    <row r="18" spans="1:14" ht="15.7">
       <c r="A18" s="15" t="s">
         <v>129</v>
       </c>
@@ -6185,11 +6714,14 @@
       <c r="L18" t="s">
         <v>825</v>
       </c>
-      <c r="M18" s="40" t="s">
+      <c r="M18" s="53" t="s">
+        <v>948</v>
+      </c>
+      <c r="N18" s="40" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.7">
+    <row r="19" spans="1:14" ht="15.7">
       <c r="A19" s="15" t="s">
         <v>133</v>
       </c>
@@ -6222,11 +6754,14 @@
       <c r="L19" t="s">
         <v>834</v>
       </c>
-      <c r="M19" s="40" t="s">
+      <c r="M19" s="53" t="s">
+        <v>949</v>
+      </c>
+      <c r="N19" s="40" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.7">
+    <row r="20" spans="1:14" ht="15.7">
       <c r="A20" s="12" t="s">
         <v>136</v>
       </c>
@@ -6261,11 +6796,14 @@
       <c r="L20" t="s">
         <v>835</v>
       </c>
-      <c r="M20" s="40" t="s">
+      <c r="M20" s="53" t="s">
+        <v>950</v>
+      </c>
+      <c r="N20" s="40" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.7">
+    <row r="21" spans="1:14" ht="15.7">
       <c r="A21" s="15" t="s">
         <v>139</v>
       </c>
@@ -6298,11 +6836,14 @@
       <c r="L21" t="s">
         <v>837</v>
       </c>
-      <c r="M21" s="40" t="s">
+      <c r="M21" s="53" t="s">
+        <v>951</v>
+      </c>
+      <c r="N21" s="40" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15.7">
+    <row r="22" spans="1:14" ht="15.7">
       <c r="A22" s="12" t="s">
         <v>142</v>
       </c>
@@ -6335,11 +6876,14 @@
       <c r="L22" t="s">
         <v>840</v>
       </c>
-      <c r="M22" s="40" t="s">
+      <c r="M22" s="53" t="s">
+        <v>952</v>
+      </c>
+      <c r="N22" s="40" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15.7">
+    <row r="23" spans="1:14" ht="15.7">
       <c r="A23" s="12" t="s">
         <v>145</v>
       </c>
@@ -6372,11 +6916,14 @@
       <c r="L23" t="s">
         <v>841</v>
       </c>
-      <c r="M23" s="40" t="s">
+      <c r="M23" s="53" t="s">
+        <v>953</v>
+      </c>
+      <c r="N23" s="40" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15.7">
+    <row r="25" spans="1:14" ht="15.7">
       <c r="A25" s="12" t="s">
         <v>154</v>
       </c>
@@ -6411,11 +6958,14 @@
       <c r="L25" t="s">
         <v>826</v>
       </c>
-      <c r="M25" s="40" t="s">
+      <c r="M25" s="53" t="s">
+        <v>954</v>
+      </c>
+      <c r="N25" s="40" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15.7">
+    <row r="26" spans="1:14" ht="15.7">
       <c r="A26" s="12" t="s">
         <v>159</v>
       </c>
@@ -6450,11 +7000,14 @@
       <c r="L26" t="s">
         <v>814</v>
       </c>
-      <c r="M26" s="40" t="s">
+      <c r="M26" s="53" t="s">
+        <v>955</v>
+      </c>
+      <c r="N26" s="40" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15.7">
+    <row r="27" spans="1:14" ht="15.7">
       <c r="A27" s="12" t="s">
         <v>162</v>
       </c>
@@ -6489,11 +7042,14 @@
       <c r="L27" t="s">
         <v>832</v>
       </c>
-      <c r="M27" s="40" t="s">
+      <c r="M27" s="53" t="s">
+        <v>956</v>
+      </c>
+      <c r="N27" s="40" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15.7">
+    <row r="28" spans="1:14" ht="15.7">
       <c r="A28" s="12" t="s">
         <v>166</v>
       </c>
@@ -6528,11 +7084,14 @@
       <c r="L28" t="s">
         <v>833</v>
       </c>
-      <c r="M28" s="40" t="s">
+      <c r="M28" s="53" t="s">
+        <v>957</v>
+      </c>
+      <c r="N28" s="40" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="15.7">
+    <row r="29" spans="1:14" ht="15.7">
       <c r="A29" s="12" t="s">
         <v>170</v>
       </c>
@@ -6567,11 +7126,14 @@
       <c r="L29" t="s">
         <v>838</v>
       </c>
-      <c r="M29" s="40" t="s">
+      <c r="M29" s="53" t="s">
+        <v>958</v>
+      </c>
+      <c r="N29" s="40" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="15.7">
+    <row r="30" spans="1:14" ht="15.7">
       <c r="A30" s="12" t="s">
         <v>174</v>
       </c>
@@ -6606,11 +7168,14 @@
       <c r="L30" t="s">
         <v>836</v>
       </c>
-      <c r="M30" s="40" t="s">
+      <c r="M30" s="53" t="s">
+        <v>959</v>
+      </c>
+      <c r="N30" s="40" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15.7">
+    <row r="31" spans="1:14" ht="15.7">
       <c r="A31" s="12" t="s">
         <v>662</v>
       </c>
@@ -6642,11 +7207,14 @@
       <c r="L31" t="s">
         <v>809</v>
       </c>
-      <c r="M31" s="40" t="s">
+      <c r="M31" s="53" t="s">
+        <v>960</v>
+      </c>
+      <c r="N31" s="40" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="15.7">
+    <row r="32" spans="1:14" ht="15.7">
       <c r="A32" s="12" t="s">
         <v>181</v>
       </c>
@@ -6679,11 +7247,14 @@
       <c r="L32" t="s">
         <v>813</v>
       </c>
-      <c r="M32" s="40" t="s">
+      <c r="M32" s="53" t="s">
+        <v>961</v>
+      </c>
+      <c r="N32" s="40" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="15.7">
+    <row r="33" spans="1:14" ht="15.7">
       <c r="A33" s="12" t="s">
         <v>184</v>
       </c>
@@ -6716,11 +7287,14 @@
       <c r="L33" t="s">
         <v>815</v>
       </c>
-      <c r="M33" s="40" t="s">
+      <c r="M33" s="53" t="s">
+        <v>962</v>
+      </c>
+      <c r="N33" s="40" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="15.7">
+    <row r="34" spans="1:14" ht="15.7">
       <c r="A34" s="12" t="s">
         <v>187</v>
       </c>
@@ -6753,11 +7327,14 @@
       <c r="L34" t="s">
         <v>827</v>
       </c>
-      <c r="M34" s="40" t="s">
+      <c r="M34" s="53" t="s">
+        <v>963</v>
+      </c>
+      <c r="N34" s="40" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="15.7">
+    <row r="35" spans="1:14" ht="15.7">
       <c r="A35" s="12" t="s">
         <v>190</v>
       </c>
@@ -6790,11 +7367,14 @@
       <c r="L35" t="s">
         <v>828</v>
       </c>
-      <c r="M35" s="40" t="s">
+      <c r="M35" s="53" t="s">
+        <v>964</v>
+      </c>
+      <c r="N35" s="40" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="15.7">
+    <row r="36" spans="1:14" ht="15.7">
       <c r="A36" s="12" t="s">
         <v>193</v>
       </c>
@@ -6827,11 +7407,14 @@
       <c r="L36" t="s">
         <v>829</v>
       </c>
-      <c r="M36" s="40" t="s">
+      <c r="M36" s="53" t="s">
+        <v>965</v>
+      </c>
+      <c r="N36" s="40" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="15.7">
+    <row r="37" spans="1:14" ht="15.7">
       <c r="A37" s="12" t="s">
         <v>196</v>
       </c>
@@ -6864,11 +7447,14 @@
       <c r="L37" t="s">
         <v>830</v>
       </c>
-      <c r="M37" s="40" t="s">
+      <c r="M37" s="53" t="s">
+        <v>966</v>
+      </c>
+      <c r="N37" s="40" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="15.7">
+    <row r="38" spans="1:14" ht="15.7">
       <c r="A38" s="12" t="s">
         <v>199</v>
       </c>
@@ -6901,11 +7487,14 @@
       <c r="L38" t="s">
         <v>831</v>
       </c>
-      <c r="M38" s="40" t="s">
+      <c r="M38" s="53" t="s">
+        <v>967</v>
+      </c>
+      <c r="N38" s="40" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="15.7">
+    <row r="39" spans="1:14" ht="15.7">
       <c r="A39" s="12" t="s">
         <v>202</v>
       </c>
@@ -6938,11 +7527,14 @@
       <c r="L39" t="s">
         <v>839</v>
       </c>
-      <c r="M39" s="40" t="s">
+      <c r="M39" s="53" t="s">
+        <v>968</v>
+      </c>
+      <c r="N39" s="40" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:14">
       <c r="A41" s="16" t="s">
         <v>287</v>
       </c>
@@ -6977,11 +7569,14 @@
       <c r="L41" t="s">
         <v>796</v>
       </c>
-      <c r="M41" t="s">
+      <c r="M41" s="53" t="s">
+        <v>969</v>
+      </c>
+      <c r="N41" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:14">
       <c r="A42" s="16" t="s">
         <v>325</v>
       </c>
@@ -7016,11 +7611,14 @@
       <c r="L42" t="s">
         <v>788</v>
       </c>
-      <c r="M42" t="s">
+      <c r="M42" s="53" t="s">
+        <v>970</v>
+      </c>
+      <c r="N42" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="43">
+    <row r="43" spans="1:14" ht="43">
       <c r="A43" s="16" t="s">
         <v>309</v>
       </c>
@@ -7053,11 +7651,14 @@
       <c r="L43" t="s">
         <v>765</v>
       </c>
-      <c r="M43" t="s">
+      <c r="M43" s="53" t="s">
+        <v>971</v>
+      </c>
+      <c r="N43" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:14">
       <c r="A44" s="20" t="s">
         <v>414</v>
       </c>
@@ -7092,11 +7693,14 @@
       <c r="L44" t="s">
         <v>789</v>
       </c>
-      <c r="M44" t="s">
+      <c r="M44" s="53" t="s">
+        <v>972</v>
+      </c>
+      <c r="N44" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:14">
       <c r="A45" s="16" t="s">
         <v>376</v>
       </c>
@@ -7131,11 +7735,14 @@
       <c r="L45" t="s">
         <v>794</v>
       </c>
-      <c r="M45" t="s">
+      <c r="M45" s="53" t="s">
+        <v>973</v>
+      </c>
+      <c r="N45" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:14">
       <c r="A46" s="20" t="s">
         <v>386</v>
       </c>
@@ -7170,11 +7777,14 @@
       <c r="L46" t="s">
         <v>772</v>
       </c>
-      <c r="M46" t="s">
+      <c r="M46" s="53" t="s">
+        <v>974</v>
+      </c>
+      <c r="N46" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="28.7">
+    <row r="47" spans="1:14" ht="28.7">
       <c r="A47" s="16" t="s">
         <v>244</v>
       </c>
@@ -7207,11 +7817,14 @@
       <c r="L47" t="s">
         <v>783</v>
       </c>
-      <c r="M47" t="s">
+      <c r="M47" s="53" t="s">
+        <v>975</v>
+      </c>
+      <c r="N47" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:14">
       <c r="A48" s="16" t="s">
         <v>228</v>
       </c>
@@ -7246,11 +7859,14 @@
       <c r="L48" t="s">
         <v>797</v>
       </c>
-      <c r="M48" t="s">
+      <c r="M48" s="53" t="s">
+        <v>976</v>
+      </c>
+      <c r="N48" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:14">
       <c r="A49" s="16" t="s">
         <v>302</v>
       </c>
@@ -7283,11 +7899,14 @@
       <c r="L49" t="s">
         <v>760</v>
       </c>
-      <c r="M49" t="s">
+      <c r="M49" s="53" t="s">
+        <v>977</v>
+      </c>
+      <c r="N49" t="s">
         <v>667</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="28.7">
+    <row r="50" spans="1:14" ht="28.7">
       <c r="A50" s="16" t="s">
         <v>352</v>
       </c>
@@ -7320,11 +7939,14 @@
       <c r="L50" t="s">
         <v>761</v>
       </c>
-      <c r="M50" t="s">
+      <c r="M50" s="53" t="s">
+        <v>978</v>
+      </c>
+      <c r="N50" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:14">
       <c r="A51" s="16" t="s">
         <v>347</v>
       </c>
@@ -7357,11 +7979,14 @@
       <c r="L51" t="s">
         <v>769</v>
       </c>
-      <c r="M51" t="s">
+      <c r="M51" s="53" t="s">
+        <v>979</v>
+      </c>
+      <c r="N51" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="28.7">
+    <row r="52" spans="1:14" ht="28.7">
       <c r="A52" s="16" t="s">
         <v>217</v>
       </c>
@@ -7393,14 +8018,17 @@
       <c r="K52">
         <v>2</v>
       </c>
-      <c r="L52" s="46" t="s">
+      <c r="L52" s="45" t="s">
         <v>758</v>
       </c>
-      <c r="M52" t="s">
+      <c r="M52" s="53" t="s">
+        <v>980</v>
+      </c>
+      <c r="N52" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="15.7">
+    <row r="53" spans="1:14" ht="15.7">
       <c r="A53" s="16" t="s">
         <v>256</v>
       </c>
@@ -7435,11 +8063,14 @@
       <c r="L53" t="s">
         <v>775</v>
       </c>
-      <c r="M53" t="s">
+      <c r="M53" s="53" t="s">
+        <v>981</v>
+      </c>
+      <c r="N53" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:14">
       <c r="A54" s="16" t="s">
         <v>380</v>
       </c>
@@ -7472,11 +8103,14 @@
       <c r="L54" t="s">
         <v>791</v>
       </c>
-      <c r="M54" t="s">
+      <c r="M54" s="53" t="s">
+        <v>982</v>
+      </c>
+      <c r="N54" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="28.7">
+    <row r="55" spans="1:14" ht="28.7">
       <c r="A55" s="16" t="s">
         <v>278</v>
       </c>
@@ -7509,11 +8143,14 @@
       <c r="L55" t="s">
         <v>768</v>
       </c>
-      <c r="M55" t="s">
+      <c r="M55" s="53" t="s">
+        <v>983</v>
+      </c>
+      <c r="N55" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="15.7">
+    <row r="56" spans="1:14" ht="15.7">
       <c r="A56" s="16" t="s">
         <v>213</v>
       </c>
@@ -7548,11 +8185,14 @@
       <c r="L56" t="s">
         <v>776</v>
       </c>
-      <c r="M56" t="s">
+      <c r="M56" s="53" t="s">
+        <v>984</v>
+      </c>
+      <c r="N56" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:14">
       <c r="A57" s="20" t="s">
         <v>389</v>
       </c>
@@ -7584,14 +8224,17 @@
       <c r="K57">
         <v>1</v>
       </c>
-      <c r="L57" s="46" t="s">
+      <c r="L57" s="45" t="s">
         <v>756</v>
       </c>
-      <c r="M57" t="s">
+      <c r="M57" s="53" t="s">
+        <v>985</v>
+      </c>
+      <c r="N57" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:14">
       <c r="A58" s="16" t="s">
         <v>378</v>
       </c>
@@ -7624,11 +8267,14 @@
       <c r="L58" t="s">
         <v>793</v>
       </c>
-      <c r="M58" t="s">
+      <c r="M58" s="53" t="s">
+        <v>986</v>
+      </c>
+      <c r="N58" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="28.7">
+    <row r="59" spans="1:14" ht="28.7">
       <c r="A59" s="16" t="s">
         <v>368</v>
       </c>
@@ -7663,11 +8309,14 @@
       <c r="L59" t="s">
         <v>803</v>
       </c>
-      <c r="M59" t="s">
+      <c r="M59" s="53" t="s">
+        <v>987</v>
+      </c>
+      <c r="N59" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:14">
       <c r="A60" s="16" t="s">
         <v>305</v>
       </c>
@@ -7702,11 +8351,14 @@
       <c r="L60" t="s">
         <v>787</v>
       </c>
-      <c r="M60" t="s">
+      <c r="M60" s="53" t="s">
+        <v>988</v>
+      </c>
+      <c r="N60" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:14">
       <c r="A61" s="16" t="s">
         <v>371</v>
       </c>
@@ -7739,11 +8391,14 @@
       <c r="L61" t="s">
         <v>802</v>
       </c>
-      <c r="M61" t="s">
+      <c r="M61" s="53" t="s">
+        <v>989</v>
+      </c>
+      <c r="N61" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="28.7">
+    <row r="62" spans="1:14" ht="28.7">
       <c r="A62" s="16" t="s">
         <v>366</v>
       </c>
@@ -7776,11 +8431,14 @@
       <c r="L62" t="s">
         <v>741</v>
       </c>
-      <c r="M62" t="s">
+      <c r="M62" s="53" t="s">
+        <v>990</v>
+      </c>
+      <c r="N62" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:14">
       <c r="A63" s="20" t="s">
         <v>403</v>
       </c>
@@ -7815,11 +8473,14 @@
       <c r="L63" t="s">
         <v>751</v>
       </c>
-      <c r="M63" t="s">
+      <c r="M63" s="53" t="s">
+        <v>991</v>
+      </c>
+      <c r="N63" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="28.7">
+    <row r="64" spans="1:14" ht="28.7">
       <c r="A64" s="16" t="s">
         <v>342</v>
       </c>
@@ -7852,11 +8513,14 @@
       <c r="L64" t="s">
         <v>777</v>
       </c>
-      <c r="M64" t="s">
+      <c r="M64" s="53" t="s">
+        <v>992</v>
+      </c>
+      <c r="N64" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:14">
       <c r="A65" s="16" t="s">
         <v>358</v>
       </c>
@@ -7889,11 +8553,14 @@
       <c r="L65" t="s">
         <v>748</v>
       </c>
-      <c r="M65" t="s">
+      <c r="M65" s="53" t="s">
+        <v>993</v>
+      </c>
+      <c r="N65" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:14">
       <c r="A66" s="16" t="s">
         <v>264</v>
       </c>
@@ -7928,11 +8595,14 @@
       <c r="L66" t="s">
         <v>801</v>
       </c>
-      <c r="M66" t="s">
+      <c r="M66" s="53" t="s">
+        <v>994</v>
+      </c>
+      <c r="N66" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="43">
+    <row r="67" spans="1:14" ht="43">
       <c r="A67" s="16" t="s">
         <v>317</v>
       </c>
@@ -7967,11 +8637,14 @@
       <c r="L67" t="s">
         <v>762</v>
       </c>
-      <c r="M67" t="s">
+      <c r="M67" s="53" t="s">
+        <v>995</v>
+      </c>
+      <c r="N67" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:14">
       <c r="A68" s="16" t="s">
         <v>329</v>
       </c>
@@ -8006,11 +8679,14 @@
       <c r="L68" t="s">
         <v>778</v>
       </c>
-      <c r="M68" t="s">
+      <c r="M68" s="53" t="s">
+        <v>996</v>
+      </c>
+      <c r="N68" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:14">
       <c r="A69" s="16" t="s">
         <v>321</v>
       </c>
@@ -8045,11 +8721,14 @@
       <c r="L69" t="s">
         <v>799</v>
       </c>
-      <c r="M69" t="s">
+      <c r="M69" s="53" t="s">
+        <v>997</v>
+      </c>
+      <c r="N69" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="28.7">
+    <row r="70" spans="1:14" ht="28.7">
       <c r="A70" s="16" t="s">
         <v>281</v>
       </c>
@@ -8082,11 +8761,14 @@
       <c r="L70" t="s">
         <v>767</v>
       </c>
-      <c r="M70" t="s">
+      <c r="M70" s="53" t="s">
+        <v>998</v>
+      </c>
+      <c r="N70" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:14">
       <c r="A71" s="16" t="s">
         <v>291</v>
       </c>
@@ -8119,11 +8801,14 @@
       <c r="L71" t="s">
         <v>795</v>
       </c>
-      <c r="M71" t="s">
+      <c r="M71" s="53" t="s">
+        <v>999</v>
+      </c>
+      <c r="N71" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:14">
       <c r="A72" s="16" t="s">
         <v>345</v>
       </c>
@@ -8158,11 +8843,14 @@
       <c r="L72" t="s">
         <v>771</v>
       </c>
-      <c r="M72" t="s">
+      <c r="M72" s="53" t="s">
+        <v>1000</v>
+      </c>
+      <c r="N72" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="28.7">
+    <row r="73" spans="1:14" ht="28.7">
       <c r="A73" s="16" t="s">
         <v>241</v>
       </c>
@@ -8195,11 +8883,14 @@
       <c r="L73" t="s">
         <v>784</v>
       </c>
-      <c r="M73" t="s">
+      <c r="M73" s="53" t="s">
+        <v>1001</v>
+      </c>
+      <c r="N73" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:14">
       <c r="A74" s="20" t="s">
         <v>408</v>
       </c>
@@ -8234,11 +8925,14 @@
       <c r="L74" t="s">
         <v>749</v>
       </c>
-      <c r="M74" t="s">
+      <c r="M74" s="53" t="s">
+        <v>1002</v>
+      </c>
+      <c r="N74" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="28.7">
+    <row r="75" spans="1:14" ht="28.7">
       <c r="A75" s="16" t="s">
         <v>360</v>
       </c>
@@ -8271,11 +8965,14 @@
       <c r="L75" t="s">
         <v>743</v>
       </c>
-      <c r="M75" t="s">
+      <c r="M75" s="53" t="s">
+        <v>1003</v>
+      </c>
+      <c r="N75" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="28.7">
+    <row r="76" spans="1:14" ht="28.7">
       <c r="A76" s="16" t="s">
         <v>246</v>
       </c>
@@ -8308,11 +9005,14 @@
       <c r="L76" t="s">
         <v>782</v>
       </c>
-      <c r="M76" t="s">
+      <c r="M76" s="53" t="s">
+        <v>1004</v>
+      </c>
+      <c r="N76" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="28.7">
+    <row r="77" spans="1:14" ht="28.7">
       <c r="A77" s="16" t="s">
         <v>238</v>
       </c>
@@ -8347,11 +9047,14 @@
       <c r="L77" t="s">
         <v>785</v>
       </c>
-      <c r="M77" t="s">
+      <c r="M77" s="53" t="s">
+        <v>1005</v>
+      </c>
+      <c r="N77" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:14">
       <c r="A78" s="16" t="s">
         <v>355</v>
       </c>
@@ -8384,11 +9087,14 @@
       <c r="L78" t="s">
         <v>759</v>
       </c>
-      <c r="M78" t="s">
+      <c r="M78" s="53" t="s">
+        <v>1006</v>
+      </c>
+      <c r="N78" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="57.35">
+    <row r="79" spans="1:14" ht="57.35">
       <c r="A79" s="16" t="s">
         <v>363</v>
       </c>
@@ -8421,11 +9127,14 @@
       <c r="L79" t="s">
         <v>742</v>
       </c>
-      <c r="M79" t="s">
+      <c r="M79" s="53" t="s">
+        <v>1007</v>
+      </c>
+      <c r="N79" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:14">
       <c r="A80" s="20" t="s">
         <v>397</v>
       </c>
@@ -8460,11 +9169,14 @@
       <c r="L80" t="s">
         <v>753</v>
       </c>
-      <c r="M80" t="s">
+      <c r="M80" s="53" t="s">
+        <v>1008</v>
+      </c>
+      <c r="N80" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:14">
       <c r="A81" s="16" t="s">
         <v>374</v>
       </c>
@@ -8497,11 +9209,14 @@
       <c r="L81" t="s">
         <v>798</v>
       </c>
-      <c r="M81" t="s">
+      <c r="M81" s="53" t="s">
+        <v>1009</v>
+      </c>
+      <c r="N81" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="28.7">
+    <row r="82" spans="1:14" ht="28.7">
       <c r="A82" s="16" t="s">
         <v>252</v>
       </c>
@@ -8534,11 +9249,14 @@
       <c r="L82" t="s">
         <v>780</v>
       </c>
-      <c r="M82" t="s">
+      <c r="M82" s="53" t="s">
+        <v>1010</v>
+      </c>
+      <c r="N82" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:14">
       <c r="A83" s="20" t="s">
         <v>406</v>
       </c>
@@ -8573,11 +9291,14 @@
       <c r="L83" t="s">
         <v>750</v>
       </c>
-      <c r="M83" t="s">
+      <c r="M83" s="53" t="s">
+        <v>1011</v>
+      </c>
+      <c r="N83" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="16.7">
+    <row r="84" spans="1:14" ht="16.7">
       <c r="A84" s="16" t="s">
         <v>259</v>
       </c>
@@ -8609,14 +9330,17 @@
       <c r="K84">
         <v>1</v>
       </c>
-      <c r="L84" s="46" t="s">
+      <c r="L84" s="45" t="s">
         <v>757</v>
       </c>
-      <c r="M84" t="s">
+      <c r="M84" s="53" t="s">
+        <v>1012</v>
+      </c>
+      <c r="N84" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="28.7">
+    <row r="85" spans="1:14" ht="28.7">
       <c r="A85" s="16" t="s">
         <v>284</v>
       </c>
@@ -8649,11 +9373,14 @@
       <c r="L85" t="s">
         <v>747</v>
       </c>
-      <c r="M85" t="s">
+      <c r="M85" s="53" t="s">
+        <v>1013</v>
+      </c>
+      <c r="N85" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:14">
       <c r="A86" s="20" t="s">
         <v>395</v>
       </c>
@@ -8685,14 +9412,17 @@
       <c r="K86">
         <v>1</v>
       </c>
-      <c r="L86" s="46" t="s">
+      <c r="L86" s="45" t="s">
         <v>754</v>
       </c>
-      <c r="M86" t="s">
+      <c r="M86" s="53" t="s">
+        <v>1014</v>
+      </c>
+      <c r="N86" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:14">
       <c r="A87" s="16" t="s">
         <v>268</v>
       </c>
@@ -8712,10 +9442,10 @@
       <c r="G87" s="25" t="s">
         <v>929</v>
       </c>
-      <c r="H87" s="51">
+      <c r="H87" s="49">
         <v>74</v>
       </c>
-      <c r="I87" s="51">
+      <c r="I87" s="49">
         <v>137</v>
       </c>
       <c r="J87">
@@ -8727,11 +9457,14 @@
       <c r="L87" t="s">
         <v>800</v>
       </c>
-      <c r="M87" t="s">
+      <c r="M87" s="53" t="s">
+        <v>1015</v>
+      </c>
+      <c r="N87" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="28.7">
+    <row r="88" spans="1:14" ht="28.7">
       <c r="A88" s="16" t="s">
         <v>349</v>
       </c>
@@ -8768,11 +9501,14 @@
       <c r="L88" t="s">
         <v>766</v>
       </c>
-      <c r="M88" t="s">
+      <c r="M88" s="53" t="s">
+        <v>1016</v>
+      </c>
+      <c r="N88" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:14">
       <c r="A89" s="16" t="s">
         <v>299</v>
       </c>
@@ -8809,11 +9545,14 @@
       <c r="L89" t="s">
         <v>774</v>
       </c>
-      <c r="M89" t="s">
+      <c r="M89" s="53" t="s">
+        <v>1017</v>
+      </c>
+      <c r="N89" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="28.7">
+    <row r="90" spans="1:14" ht="28.7">
       <c r="A90" s="16" t="s">
         <v>254</v>
       </c>
@@ -8848,11 +9587,14 @@
       <c r="L90" t="s">
         <v>779</v>
       </c>
-      <c r="M90" t="s">
+      <c r="M90" s="53" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N90" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:14">
       <c r="A91" s="16" t="s">
         <v>275</v>
       </c>
@@ -8885,11 +9627,14 @@
       <c r="L91" t="s">
         <v>770</v>
       </c>
-      <c r="M91" t="s">
+      <c r="M91" s="53" t="s">
+        <v>1019</v>
+      </c>
+      <c r="N91" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="43">
+    <row r="92" spans="1:14" ht="43">
       <c r="A92" s="16" t="s">
         <v>312</v>
       </c>
@@ -8924,11 +9669,14 @@
       <c r="L92" t="s">
         <v>764</v>
       </c>
-      <c r="M92" t="s">
+      <c r="M92" s="53" t="s">
+        <v>1020</v>
+      </c>
+      <c r="N92" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="43">
+    <row r="93" spans="1:14" ht="43">
       <c r="A93" s="16" t="s">
         <v>315</v>
       </c>
@@ -8963,11 +9711,14 @@
       <c r="L93" t="s">
         <v>763</v>
       </c>
-      <c r="M93" t="s">
+      <c r="M93" s="53" t="s">
+        <v>1021</v>
+      </c>
+      <c r="N93" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:14">
       <c r="A94" s="20" t="s">
         <v>382</v>
       </c>
@@ -9002,11 +9753,14 @@
       <c r="L94" t="s">
         <v>773</v>
       </c>
-      <c r="M94" t="s">
+      <c r="M94" s="53" t="s">
+        <v>1022</v>
+      </c>
+      <c r="N94" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:14">
       <c r="A95" s="20" t="s">
         <v>393</v>
       </c>
@@ -9038,14 +9792,17 @@
       <c r="K95">
         <v>1</v>
       </c>
-      <c r="L95" s="46" t="s">
+      <c r="L95" s="45" t="s">
         <v>755</v>
       </c>
-      <c r="M95" t="s">
+      <c r="M95" s="53" t="s">
+        <v>1023</v>
+      </c>
+      <c r="N95" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:14">
       <c r="A96" s="20" t="s">
         <v>399</v>
       </c>
@@ -9080,11 +9837,14 @@
       <c r="L96" t="s">
         <v>752</v>
       </c>
-      <c r="M96" t="s">
+      <c r="M96" s="53" t="s">
+        <v>1024</v>
+      </c>
+      <c r="N96" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="28.7">
+    <row r="97" spans="1:14" ht="28.7">
       <c r="A97" s="16" t="s">
         <v>224</v>
       </c>
@@ -9119,11 +9879,14 @@
       <c r="L97" t="s">
         <v>744</v>
       </c>
-      <c r="M97" t="s">
+      <c r="M97" s="53" t="s">
+        <v>1025</v>
+      </c>
+      <c r="N97" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:14">
       <c r="A98" s="20" t="s">
         <v>410</v>
       </c>
@@ -9158,11 +9921,14 @@
       <c r="L98" t="s">
         <v>790</v>
       </c>
-      <c r="M98" t="s">
+      <c r="M98" s="53" t="s">
+        <v>1026</v>
+      </c>
+      <c r="N98" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="99" spans="1:13">
+    <row r="99" spans="1:14">
       <c r="A99" s="16" t="s">
         <v>319</v>
       </c>
@@ -9195,11 +9961,14 @@
       <c r="L99" t="s">
         <v>746</v>
       </c>
-      <c r="M99" t="s">
+      <c r="M99" s="53" t="s">
+        <v>1027</v>
+      </c>
+      <c r="N99" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="28.7">
+    <row r="100" spans="1:14" ht="28.7">
       <c r="A100" s="16" t="s">
         <v>235</v>
       </c>
@@ -9232,11 +10001,14 @@
       <c r="L100" t="s">
         <v>786</v>
       </c>
-      <c r="M100" t="s">
+      <c r="M100" s="53" t="s">
+        <v>1028</v>
+      </c>
+      <c r="N100" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:14">
       <c r="A101" s="16" t="s">
         <v>294</v>
       </c>
@@ -9269,11 +10041,14 @@
       <c r="L101" t="s">
         <v>792</v>
       </c>
-      <c r="M101" t="s">
+      <c r="M101" s="53" t="s">
+        <v>1029</v>
+      </c>
+      <c r="N101" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="102" spans="1:13" ht="43">
+    <row r="102" spans="1:14" ht="43">
       <c r="A102" s="16" t="s">
         <v>249</v>
       </c>
@@ -9306,11 +10081,14 @@
       <c r="L102" t="s">
         <v>781</v>
       </c>
-      <c r="M102" t="s">
+      <c r="M102" s="53" t="s">
+        <v>1030</v>
+      </c>
+      <c r="N102" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="103" spans="1:13" ht="100.35">
+    <row r="103" spans="1:14" ht="100.35">
       <c r="A103" s="16" t="s">
         <v>220</v>
       </c>
@@ -9345,11 +10123,14 @@
       <c r="L103" t="s">
         <v>745</v>
       </c>
-      <c r="M103" t="s">
+      <c r="M103" s="53" t="s">
+        <v>1031</v>
+      </c>
+      <c r="N103" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:14">
       <c r="A104" s="16" t="s">
         <v>261</v>
       </c>
@@ -9382,11 +10163,14 @@
       <c r="L104" t="s">
         <v>804</v>
       </c>
-      <c r="M104" t="s">
+      <c r="M104" s="53" t="s">
+        <v>1032</v>
+      </c>
+      <c r="N104" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:14">
       <c r="A105" s="21" t="s">
         <v>178</v>
       </c>
@@ -9419,11 +10203,14 @@
       <c r="L105" t="s">
         <v>842</v>
       </c>
-      <c r="M105" t="s">
+      <c r="M105" s="53" t="s">
+        <v>1033</v>
+      </c>
+      <c r="N105" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:14">
       <c r="A106" s="21" t="s">
         <v>592</v>
       </c>
@@ -9458,11 +10245,14 @@
       <c r="L106" t="s">
         <v>843</v>
       </c>
-      <c r="M106" t="s">
+      <c r="M106" s="53" t="s">
+        <v>1034</v>
+      </c>
+      <c r="N106" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="28.7">
+    <row r="107" spans="1:14" ht="28.7">
       <c r="A107" s="21" t="s">
         <v>418</v>
       </c>
@@ -9495,11 +10285,14 @@
       <c r="L107" t="s">
         <v>844</v>
       </c>
-      <c r="M107" s="22" t="s">
+      <c r="M107" s="53" t="s">
+        <v>1035</v>
+      </c>
+      <c r="N107" s="22" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="108" spans="1:13">
+    <row r="108" spans="1:14">
       <c r="A108" s="21" t="s">
         <v>542</v>
       </c>
@@ -9534,11 +10327,14 @@
       <c r="L108" t="s">
         <v>845</v>
       </c>
-      <c r="M108" t="s">
+      <c r="M108" s="53" t="s">
+        <v>1036</v>
+      </c>
+      <c r="N108" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="109" spans="1:13">
+    <row r="109" spans="1:14">
       <c r="A109" s="21" t="s">
         <v>586</v>
       </c>
@@ -9573,11 +10369,14 @@
       <c r="L109" t="s">
         <v>846</v>
       </c>
-      <c r="M109" t="s">
+      <c r="M109" s="53" t="s">
+        <v>1037</v>
+      </c>
+      <c r="N109" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="110" spans="1:13">
+    <row r="110" spans="1:14">
       <c r="A110" s="21" t="s">
         <v>489</v>
       </c>
@@ -9610,11 +10409,14 @@
       <c r="L110" t="s">
         <v>847</v>
       </c>
-      <c r="M110" t="s">
+      <c r="M110" s="53" t="s">
+        <v>1038</v>
+      </c>
+      <c r="N110" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="28.7">
+    <row r="111" spans="1:14" ht="28.7">
       <c r="A111" s="21" t="s">
         <v>491</v>
       </c>
@@ -9649,11 +10451,14 @@
       <c r="L111" t="s">
         <v>848</v>
       </c>
-      <c r="M111" t="s">
+      <c r="M111" s="53" t="s">
+        <v>1039</v>
+      </c>
+      <c r="N111" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="112" spans="1:13">
+    <row r="112" spans="1:14">
       <c r="A112" s="21" t="s">
         <v>522</v>
       </c>
@@ -9688,11 +10493,14 @@
       <c r="L112" t="s">
         <v>849</v>
       </c>
-      <c r="M112" t="s">
+      <c r="M112" s="53" t="s">
+        <v>1040</v>
+      </c>
+      <c r="N112" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="113" spans="1:13">
+    <row r="113" spans="1:14">
       <c r="A113" s="21" t="s">
         <v>421</v>
       </c>
@@ -9725,11 +10533,14 @@
       <c r="L113" t="s">
         <v>850</v>
       </c>
-      <c r="M113" s="22" t="s">
+      <c r="M113" s="53" t="s">
+        <v>1041</v>
+      </c>
+      <c r="N113" s="22" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="114" spans="1:13">
+    <row r="114" spans="1:14">
       <c r="A114" s="21" t="s">
         <v>532</v>
       </c>
@@ -9763,14 +10574,17 @@
       <c r="K114">
         <v>1</v>
       </c>
-      <c r="L114" s="52" t="s">
+      <c r="L114" s="50" t="s">
         <v>851</v>
       </c>
-      <c r="M114" t="s">
+      <c r="M114" s="53" t="s">
+        <v>1042</v>
+      </c>
+      <c r="N114" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="115" spans="1:13">
+    <row r="115" spans="1:14">
       <c r="A115" s="21" t="s">
         <v>468</v>
       </c>
@@ -9803,12 +10617,15 @@
       <c r="L115" t="s">
         <v>852</v>
       </c>
-      <c r="M115" t="s">
+      <c r="M115" s="53" t="s">
+        <v>1043</v>
+      </c>
+      <c r="N115" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="116" spans="1:13">
-      <c r="A116" s="50" t="s">
+    <row r="116" spans="1:14">
+      <c r="A116" s="48" t="s">
         <v>483</v>
       </c>
       <c r="B116" s="24" t="s">
@@ -9840,11 +10657,14 @@
       <c r="L116" t="s">
         <v>853</v>
       </c>
-      <c r="M116" t="s">
+      <c r="M116" s="53" t="s">
+        <v>1044</v>
+      </c>
+      <c r="N116" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="117" spans="1:13">
+    <row r="117" spans="1:14">
       <c r="A117" s="26" t="s">
         <v>605</v>
       </c>
@@ -9875,11 +10695,14 @@
       <c r="L117" t="s">
         <v>854</v>
       </c>
-      <c r="M117" t="s">
+      <c r="M117" s="53" t="s">
+        <v>1045</v>
+      </c>
+      <c r="N117" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="118" spans="1:13">
+    <row r="118" spans="1:14">
       <c r="A118" s="21" t="s">
         <v>471</v>
       </c>
@@ -9912,11 +10735,14 @@
       <c r="L118" t="s">
         <v>855</v>
       </c>
-      <c r="M118" t="s">
+      <c r="M118" s="53" t="s">
+        <v>1046</v>
+      </c>
+      <c r="N118" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="119" spans="1:13">
+    <row r="119" spans="1:14">
       <c r="A119" s="21" t="s">
         <v>473</v>
       </c>
@@ -9951,11 +10777,14 @@
       <c r="L119" t="s">
         <v>856</v>
       </c>
-      <c r="M119" t="s">
+      <c r="M119" s="53" t="s">
+        <v>1047</v>
+      </c>
+      <c r="N119" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="120" spans="1:13">
+    <row r="120" spans="1:14">
       <c r="A120" s="21" t="s">
         <v>101</v>
       </c>
@@ -9992,11 +10821,14 @@
       <c r="L120" t="s">
         <v>857</v>
       </c>
-      <c r="M120" t="s">
+      <c r="M120" s="53" t="s">
+        <v>1048</v>
+      </c>
+      <c r="N120" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="121" spans="1:13">
+    <row r="121" spans="1:14">
       <c r="A121" s="21" t="s">
         <v>544</v>
       </c>
@@ -10031,11 +10863,14 @@
       <c r="L121" t="s">
         <v>858</v>
       </c>
-      <c r="M121" t="s">
+      <c r="M121" s="53" t="s">
+        <v>1049</v>
+      </c>
+      <c r="N121" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="122" spans="1:13">
+    <row r="122" spans="1:14">
       <c r="A122" s="21" t="s">
         <v>547</v>
       </c>
@@ -10070,11 +10905,14 @@
       <c r="L122" t="s">
         <v>859</v>
       </c>
-      <c r="M122" t="s">
+      <c r="M122" s="53" t="s">
+        <v>1050</v>
+      </c>
+      <c r="N122" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="123" spans="1:13">
+    <row r="123" spans="1:14">
       <c r="A123" s="21" t="s">
         <v>550</v>
       </c>
@@ -10109,11 +10947,14 @@
       <c r="L123" t="s">
         <v>860</v>
       </c>
-      <c r="M123" t="s">
+      <c r="M123" s="53" t="s">
+        <v>1051</v>
+      </c>
+      <c r="N123" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="124" spans="1:13">
+    <row r="124" spans="1:14">
       <c r="A124" s="21" t="s">
         <v>553</v>
       </c>
@@ -10146,11 +10987,14 @@
       <c r="L124" t="s">
         <v>861</v>
       </c>
-      <c r="M124" t="s">
+      <c r="M124" s="53" t="s">
+        <v>1052</v>
+      </c>
+      <c r="N124" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="125" spans="1:13">
+    <row r="125" spans="1:14">
       <c r="A125" s="21" t="s">
         <v>556</v>
       </c>
@@ -10185,11 +11029,14 @@
       <c r="L125" t="s">
         <v>862</v>
       </c>
-      <c r="M125" t="s">
+      <c r="M125" s="53" t="s">
+        <v>1053</v>
+      </c>
+      <c r="N125" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="126" spans="1:13">
+    <row r="126" spans="1:14">
       <c r="A126" s="21" t="s">
         <v>494</v>
       </c>
@@ -10224,11 +11071,14 @@
       <c r="L126" t="s">
         <v>863</v>
       </c>
-      <c r="M126" s="24" t="s">
+      <c r="M126" s="53" t="s">
+        <v>1054</v>
+      </c>
+      <c r="N126" s="24" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="127" spans="1:13">
+    <row r="127" spans="1:14">
       <c r="A127" s="21" t="s">
         <v>497</v>
       </c>
@@ -10263,11 +11113,14 @@
       <c r="L127" t="s">
         <v>864</v>
       </c>
-      <c r="M127" t="s">
+      <c r="M127" s="53" t="s">
+        <v>1055</v>
+      </c>
+      <c r="N127" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="128" spans="1:13" ht="28.7">
+    <row r="128" spans="1:14" ht="28.7">
       <c r="A128" s="21" t="s">
         <v>511</v>
       </c>
@@ -10302,11 +11155,14 @@
       <c r="L128" t="s">
         <v>865</v>
       </c>
-      <c r="M128" t="s">
+      <c r="M128" s="53" t="s">
+        <v>1056</v>
+      </c>
+      <c r="N128" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="129" spans="1:13" ht="28.7">
+    <row r="129" spans="1:14" ht="28.7">
       <c r="A129" s="21" t="s">
         <v>583</v>
       </c>
@@ -10339,11 +11195,14 @@
       <c r="L129" t="s">
         <v>866</v>
       </c>
-      <c r="M129" t="s">
+      <c r="M129" s="53" t="s">
+        <v>1057</v>
+      </c>
+      <c r="N129" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="130" spans="1:13">
+    <row r="130" spans="1:14">
       <c r="A130" s="21" t="s">
         <v>424</v>
       </c>
@@ -10376,11 +11235,14 @@
       <c r="L130" t="s">
         <v>867</v>
       </c>
-      <c r="M130" t="s">
+      <c r="M130" s="53" t="s">
+        <v>1058</v>
+      </c>
+      <c r="N130" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="28.7">
+    <row r="131" spans="1:14" ht="28.7">
       <c r="A131" s="21" t="s">
         <v>427</v>
       </c>
@@ -10413,11 +11275,14 @@
       <c r="L131" t="s">
         <v>868</v>
       </c>
-      <c r="M131" s="22" t="s">
+      <c r="M131" s="53" t="s">
+        <v>1059</v>
+      </c>
+      <c r="N131" s="22" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="132" spans="1:13">
+    <row r="132" spans="1:14">
       <c r="A132" s="21" t="s">
         <v>430</v>
       </c>
@@ -10450,11 +11315,14 @@
       <c r="L132" t="s">
         <v>869</v>
       </c>
-      <c r="M132" s="22" t="s">
+      <c r="M132" s="53" t="s">
+        <v>1060</v>
+      </c>
+      <c r="N132" s="22" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="133" spans="1:13">
+    <row r="133" spans="1:14">
       <c r="A133" s="21" t="s">
         <v>589</v>
       </c>
@@ -10491,11 +11359,14 @@
       <c r="L133" t="s">
         <v>870</v>
       </c>
-      <c r="M133" t="s">
+      <c r="M133" s="53" t="s">
+        <v>1061</v>
+      </c>
+      <c r="N133" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="134" spans="1:13" ht="28.7">
+    <row r="134" spans="1:14" ht="28.7">
       <c r="A134" s="21" t="s">
         <v>433</v>
       </c>
@@ -10528,11 +11399,14 @@
       <c r="L134" t="s">
         <v>871</v>
       </c>
-      <c r="M134" s="22" t="s">
+      <c r="M134" s="53" t="s">
+        <v>1062</v>
+      </c>
+      <c r="N134" s="22" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="135" spans="1:13">
+    <row r="135" spans="1:14">
       <c r="A135" s="21" t="s">
         <v>435</v>
       </c>
@@ -10565,11 +11439,14 @@
       <c r="L135" t="s">
         <v>872</v>
       </c>
-      <c r="M135" t="s">
+      <c r="M135" s="53" t="s">
+        <v>1063</v>
+      </c>
+      <c r="N135" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="136" spans="1:13">
+    <row r="136" spans="1:14">
       <c r="A136" s="21" t="s">
         <v>438</v>
       </c>
@@ -10602,11 +11479,14 @@
       <c r="L136" t="s">
         <v>873</v>
       </c>
-      <c r="M136" t="s">
+      <c r="M136" s="53" t="s">
+        <v>1064</v>
+      </c>
+      <c r="N136" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="137" spans="1:13">
+    <row r="137" spans="1:14">
       <c r="A137" s="21" t="s">
         <v>560</v>
       </c>
@@ -10639,11 +11519,14 @@
       <c r="L137" t="s">
         <v>874</v>
       </c>
-      <c r="M137" t="s">
+      <c r="M137" s="53" t="s">
+        <v>1065</v>
+      </c>
+      <c r="N137" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="138" spans="1:13">
+    <row r="138" spans="1:14">
       <c r="A138" s="21" t="s">
         <v>563</v>
       </c>
@@ -10676,11 +11559,14 @@
       <c r="L138" t="s">
         <v>875</v>
       </c>
-      <c r="M138" t="s">
+      <c r="M138" s="53" t="s">
+        <v>1066</v>
+      </c>
+      <c r="N138" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="139" spans="1:13">
+    <row r="139" spans="1:14">
       <c r="A139" s="21" t="s">
         <v>566</v>
       </c>
@@ -10715,11 +11601,14 @@
       <c r="L139" t="s">
         <v>876</v>
       </c>
-      <c r="M139" t="s">
+      <c r="M139" s="53" t="s">
+        <v>1067</v>
+      </c>
+      <c r="N139" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="140" spans="1:13">
+    <row r="140" spans="1:14">
       <c r="A140" s="21" t="s">
         <v>570</v>
       </c>
@@ -10752,11 +11641,14 @@
       <c r="L140" t="s">
         <v>877</v>
       </c>
-      <c r="M140" t="s">
+      <c r="M140" s="53" t="s">
+        <v>1068</v>
+      </c>
+      <c r="N140" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="141" spans="1:13">
+    <row r="141" spans="1:14">
       <c r="A141" s="21" t="s">
         <v>441</v>
       </c>
@@ -10793,11 +11685,14 @@
       <c r="L141" t="s">
         <v>878</v>
       </c>
-      <c r="M141" s="22" t="s">
+      <c r="M141" s="53" t="s">
+        <v>1069</v>
+      </c>
+      <c r="N141" s="22" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="142" spans="1:13" ht="28.7">
+    <row r="142" spans="1:14" ht="28.7">
       <c r="A142" s="21" t="s">
         <v>476</v>
       </c>
@@ -10832,11 +11727,14 @@
       <c r="L142" t="s">
         <v>879</v>
       </c>
-      <c r="M142" t="s">
+      <c r="M142" s="53" t="s">
+        <v>1070</v>
+      </c>
+      <c r="N142" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="143" spans="1:13">
+    <row r="143" spans="1:14">
       <c r="A143" s="21" t="s">
         <v>526</v>
       </c>
@@ -10869,11 +11767,14 @@
       <c r="L143" t="s">
         <v>880</v>
       </c>
-      <c r="M143" t="s">
+      <c r="M143" s="53" t="s">
+        <v>1071</v>
+      </c>
+      <c r="N143" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="144" spans="1:13">
+    <row r="144" spans="1:14">
       <c r="A144" s="21" t="s">
         <v>573</v>
       </c>
@@ -10906,11 +11807,14 @@
       <c r="L144" t="s">
         <v>881</v>
       </c>
-      <c r="M144" t="s">
+      <c r="M144" s="53" t="s">
+        <v>1072</v>
+      </c>
+      <c r="N144" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="145" spans="1:13">
+    <row r="145" spans="1:14">
       <c r="A145" s="21" t="s">
         <v>576</v>
       </c>
@@ -10945,11 +11849,14 @@
       <c r="L145" t="s">
         <v>882</v>
       </c>
-      <c r="M145" t="s">
+      <c r="M145" s="53" t="s">
+        <v>1073</v>
+      </c>
+      <c r="N145" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="146" spans="1:13">
+    <row r="146" spans="1:14">
       <c r="A146" s="21" t="s">
         <v>580</v>
       </c>
@@ -10984,11 +11891,14 @@
       <c r="L146" t="s">
         <v>883</v>
       </c>
-      <c r="M146" t="s">
+      <c r="M146" s="53" t="s">
+        <v>1074</v>
+      </c>
+      <c r="N146" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="147" spans="1:13">
+    <row r="147" spans="1:14">
       <c r="A147" s="21" t="s">
         <v>535</v>
       </c>
@@ -11023,11 +11933,14 @@
       <c r="L147" t="s">
         <v>884</v>
       </c>
-      <c r="M147" t="s">
+      <c r="M147" s="53" t="s">
+        <v>1075</v>
+      </c>
+      <c r="N147" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="148" spans="1:13">
+    <row r="148" spans="1:14">
       <c r="A148" s="21" t="s">
         <v>539</v>
       </c>
@@ -11057,14 +11970,17 @@
       <c r="K148">
         <v>1</v>
       </c>
-      <c r="L148" s="52" t="s">
+      <c r="L148" s="50" t="s">
         <v>885</v>
       </c>
-      <c r="M148" t="s">
+      <c r="M148" s="53" t="s">
+        <v>1076</v>
+      </c>
+      <c r="N148" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="149" spans="1:13" ht="28.7">
+    <row r="149" spans="1:14" ht="28.7">
       <c r="A149" s="21" t="s">
         <v>499</v>
       </c>
@@ -11099,11 +12015,14 @@
       <c r="L149" t="s">
         <v>887</v>
       </c>
-      <c r="M149" t="s">
+      <c r="M149" s="53" t="s">
+        <v>1077</v>
+      </c>
+      <c r="N149" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="150" spans="1:13">
+    <row r="150" spans="1:14">
       <c r="A150" s="21" t="s">
         <v>444</v>
       </c>
@@ -11138,11 +12057,14 @@
       <c r="L150" t="s">
         <v>888</v>
       </c>
-      <c r="M150" t="s">
+      <c r="M150" s="53" t="s">
+        <v>1078</v>
+      </c>
+      <c r="N150" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="151" spans="1:13">
+    <row r="151" spans="1:14">
       <c r="A151" s="21" t="s">
         <v>447</v>
       </c>
@@ -11175,11 +12097,14 @@
       <c r="L151" t="s">
         <v>889</v>
       </c>
-      <c r="M151" s="22" t="s">
+      <c r="M151" s="53" t="s">
+        <v>1079</v>
+      </c>
+      <c r="N151" s="22" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="152" spans="1:13">
+    <row r="152" spans="1:14">
       <c r="A152" s="21" t="s">
         <v>528</v>
       </c>
@@ -11214,11 +12139,14 @@
       <c r="L152" t="s">
         <v>890</v>
       </c>
-      <c r="M152" t="s">
+      <c r="M152" s="53" t="s">
+        <v>1080</v>
+      </c>
+      <c r="N152" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="153" spans="1:13">
+    <row r="153" spans="1:14">
       <c r="A153" s="21" t="s">
         <v>517</v>
       </c>
@@ -11253,11 +12181,14 @@
       <c r="L153" t="s">
         <v>891</v>
       </c>
-      <c r="M153" t="s">
+      <c r="M153" s="53" t="s">
+        <v>1081</v>
+      </c>
+      <c r="N153" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="154" spans="1:13">
+    <row r="154" spans="1:14">
       <c r="A154" s="21" t="s">
         <v>514</v>
       </c>
@@ -11292,11 +12223,14 @@
       <c r="L154" t="s">
         <v>892</v>
       </c>
-      <c r="M154" t="s">
+      <c r="M154" s="53" t="s">
+        <v>1082</v>
+      </c>
+      <c r="N154" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="155" spans="1:13">
+    <row r="155" spans="1:14">
       <c r="A155" s="21" t="s">
         <v>530</v>
       </c>
@@ -11314,13 +12248,13 @@
       <c r="G155" s="25" t="s">
         <v>931</v>
       </c>
-      <c r="H155" s="51">
+      <c r="H155" s="49">
         <v>18.399999999999999</v>
       </c>
-      <c r="I155" s="51">
+      <c r="I155" s="49">
         <v>29.3</v>
       </c>
-      <c r="J155" s="51">
+      <c r="J155" s="49">
         <v>14.6</v>
       </c>
       <c r="K155">
@@ -11329,11 +12263,14 @@
       <c r="L155" t="s">
         <v>893</v>
       </c>
-      <c r="M155" t="s">
+      <c r="M155" s="53" t="s">
+        <v>1083</v>
+      </c>
+      <c r="N155" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="156" spans="1:13" ht="28.7">
+    <row r="156" spans="1:14" ht="28.7">
       <c r="A156" s="21" t="s">
         <v>479</v>
       </c>
@@ -11366,11 +12303,14 @@
       <c r="L156" t="s">
         <v>894</v>
       </c>
-      <c r="M156" t="s">
+      <c r="M156" s="53" t="s">
+        <v>1084</v>
+      </c>
+      <c r="N156" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="28.7">
+    <row r="157" spans="1:14" ht="28.7">
       <c r="A157" s="21" t="s">
         <v>520</v>
       </c>
@@ -11403,11 +12343,14 @@
       <c r="L157" t="s">
         <v>895</v>
       </c>
-      <c r="M157" t="s">
+      <c r="M157" s="53" t="s">
+        <v>1085</v>
+      </c>
+      <c r="N157" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="158" spans="1:13">
+    <row r="158" spans="1:14">
       <c r="A158" s="21" t="s">
         <v>486</v>
       </c>
@@ -11440,11 +12383,14 @@
       <c r="L158" t="s">
         <v>896</v>
       </c>
-      <c r="M158" t="s">
+      <c r="M158" s="53" t="s">
+        <v>1086</v>
+      </c>
+      <c r="N158" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="159" spans="1:13">
+    <row r="159" spans="1:14">
       <c r="A159" s="21" t="s">
         <v>450</v>
       </c>
@@ -11477,11 +12423,14 @@
       <c r="L159" t="s">
         <v>897</v>
       </c>
-      <c r="M159" t="s">
+      <c r="M159" s="53" t="s">
+        <v>1087</v>
+      </c>
+      <c r="N159" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="160" spans="1:13">
+    <row r="160" spans="1:14">
       <c r="A160" s="21" t="s">
         <v>453</v>
       </c>
@@ -11514,11 +12463,14 @@
       <c r="L160" t="s">
         <v>898</v>
       </c>
-      <c r="M160" s="22" t="s">
+      <c r="M160" s="53" t="s">
+        <v>1088</v>
+      </c>
+      <c r="N160" s="22" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="161" spans="1:13">
+    <row r="161" spans="1:14">
       <c r="A161" s="21" t="s">
         <v>456</v>
       </c>
@@ -11551,11 +12503,14 @@
       <c r="L161" t="s">
         <v>899</v>
       </c>
-      <c r="M161" s="22" t="s">
+      <c r="M161" s="53" t="s">
+        <v>1089</v>
+      </c>
+      <c r="N161" s="22" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="162" spans="1:13" ht="28.7">
+    <row r="162" spans="1:14" ht="28.7">
       <c r="A162" s="21" t="s">
         <v>149</v>
       </c>
@@ -11588,11 +12543,14 @@
       <c r="L162" t="s">
         <v>900</v>
       </c>
-      <c r="M162" t="s">
+      <c r="M162" s="53" t="s">
+        <v>1090</v>
+      </c>
+      <c r="N162" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="163" spans="1:13">
+    <row r="163" spans="1:14">
       <c r="A163" s="26" t="s">
         <v>608</v>
       </c>
@@ -11623,11 +12581,14 @@
       <c r="L163" t="s">
         <v>901</v>
       </c>
-      <c r="M163" t="s">
+      <c r="M163" s="53" t="s">
+        <v>1091</v>
+      </c>
+      <c r="N163" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="164" spans="1:13">
+    <row r="164" spans="1:14">
       <c r="A164" s="26" t="s">
         <v>611</v>
       </c>
@@ -11655,14 +12616,17 @@
       <c r="K164">
         <v>1</v>
       </c>
-      <c r="L164" s="52" t="s">
+      <c r="L164" s="50" t="s">
         <v>886</v>
       </c>
-      <c r="M164" t="s">
+      <c r="M164" s="53" t="s">
+        <v>1092</v>
+      </c>
+      <c r="N164" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="165" spans="1:13">
+    <row r="165" spans="1:14">
       <c r="A165" s="21" t="s">
         <v>458</v>
       </c>
@@ -11692,12 +12656,12 @@
       <c r="K165">
         <v>1</v>
       </c>
-      <c r="L165" s="53"/>
-      <c r="M165" t="s">
+      <c r="L165" s="51"/>
+      <c r="N165" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="166" spans="1:13">
+    <row r="166" spans="1:14">
       <c r="A166" s="16" t="s">
         <v>335</v>
       </c>
@@ -11729,12 +12693,12 @@
       <c r="K166">
         <v>1</v>
       </c>
-      <c r="L166" s="54"/>
-      <c r="M166" t="s">
+      <c r="L166" s="52"/>
+      <c r="N166" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="167" spans="1:13">
+    <row r="167" spans="1:14">
       <c r="A167" s="16" t="s">
         <v>232</v>
       </c>
@@ -11766,12 +12730,12 @@
       <c r="K167">
         <v>2</v>
       </c>
-      <c r="L167" s="54"/>
-      <c r="M167" t="s">
+      <c r="L167" s="52"/>
+      <c r="N167" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="168" spans="1:13">
+    <row r="168" spans="1:14">
       <c r="A168" s="16" t="s">
         <v>296</v>
       </c>
@@ -11801,12 +12765,12 @@
       <c r="K168">
         <v>4</v>
       </c>
-      <c r="L168" s="54"/>
-      <c r="M168" t="s">
+      <c r="L168" s="52"/>
+      <c r="N168" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="169" spans="1:13">
+    <row r="169" spans="1:14">
       <c r="A169" s="16" t="s">
         <v>332</v>
       </c>
@@ -11836,12 +12800,12 @@
       <c r="K169">
         <v>1</v>
       </c>
-      <c r="L169" s="54"/>
-      <c r="M169" t="s">
+      <c r="L169" s="52"/>
+      <c r="N169" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="170" spans="1:13" ht="28.7">
+    <row r="170" spans="1:14" ht="28.7">
       <c r="A170" s="16" t="s">
         <v>339</v>
       </c>
@@ -11871,12 +12835,12 @@
       <c r="K170">
         <v>1</v>
       </c>
-      <c r="L170" s="54"/>
-      <c r="M170" t="s">
+      <c r="L170" s="52"/>
+      <c r="N170" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="171" spans="1:13">
+    <row r="171" spans="1:14">
       <c r="A171" s="21" t="s">
         <v>461</v>
       </c>
@@ -11906,12 +12870,12 @@
       <c r="K171">
         <v>1</v>
       </c>
-      <c r="L171" s="54"/>
-      <c r="M171" s="22" t="s">
+      <c r="L171" s="52"/>
+      <c r="N171" s="22" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="172" spans="1:13" ht="28.7">
+    <row r="172" spans="1:14" ht="28.7">
       <c r="A172" s="21" t="s">
         <v>502</v>
       </c>
@@ -11943,12 +12907,12 @@
       <c r="K172">
         <v>1</v>
       </c>
-      <c r="L172" s="54"/>
-      <c r="M172" t="s">
+      <c r="L172" s="52"/>
+      <c r="N172" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="173" spans="1:13">
+    <row r="173" spans="1:14">
       <c r="A173" s="16" t="s">
         <v>271</v>
       </c>
@@ -11980,12 +12944,12 @@
       <c r="K173">
         <v>1</v>
       </c>
-      <c r="L173" s="54"/>
-      <c r="M173" t="s">
+      <c r="L173" s="52"/>
+      <c r="N173" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="174" spans="1:13" ht="28.7">
+    <row r="174" spans="1:14" ht="28.7">
       <c r="A174" s="21" t="s">
         <v>506</v>
       </c>
@@ -12017,12 +12981,12 @@
       <c r="K174">
         <v>1</v>
       </c>
-      <c r="L174" s="54"/>
-      <c r="M174" t="s">
+      <c r="L174" s="52"/>
+      <c r="N174" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="175" spans="1:13" ht="28.7">
+    <row r="175" spans="1:14" ht="28.7">
       <c r="A175" s="21" t="s">
         <v>509</v>
       </c>
@@ -12054,12 +13018,12 @@
       <c r="K175">
         <v>1</v>
       </c>
-      <c r="L175" s="54"/>
-      <c r="M175" t="s">
+      <c r="L175" s="52"/>
+      <c r="N175" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="176" spans="1:13">
+    <row r="176" spans="1:14">
       <c r="A176" s="23" t="s">
         <v>463</v>
       </c>
@@ -12089,12 +13053,12 @@
       <c r="K176">
         <v>2</v>
       </c>
-      <c r="L176" s="54"/>
-      <c r="M176" s="22" t="s">
+      <c r="L176" s="52"/>
+      <c r="N176" s="22" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="177" spans="1:13">
+    <row r="177" spans="1:14">
       <c r="A177" s="23" t="s">
         <v>466</v>
       </c>
@@ -12124,16 +13088,16 @@
       <c r="K177">
         <v>2</v>
       </c>
-      <c r="L177" s="54"/>
-      <c r="M177" s="22" t="s">
+      <c r="L177" s="52"/>
+      <c r="N177" s="22" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="178" spans="1:13">
-      <c r="M178" s="22"/>
+    <row r="178" spans="1:14">
+      <c r="N178" s="22"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:M183">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A41:N183">
     <sortCondition ref="L41:L183"/>
     <sortCondition ref="A41:A183"/>
   </sortState>
@@ -14709,7 +15673,7 @@
   <cols>
     <col min="1" max="1" width="8.9375" style="1"/>
     <col min="2" max="2" width="8.9375" customWidth="1"/>
-    <col min="3" max="3" width="12" style="46" customWidth="1"/>
+    <col min="3" max="3" width="12" style="45" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -14719,7 +15683,7 @@
       <c r="B1" t="s">
         <v>690</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="45" t="s">
         <v>689</v>
       </c>
     </row>
@@ -14727,7 +15691,7 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" t="s">
         <v>715</v>
       </c>
     </row>
@@ -14738,7 +15702,7 @@
       <c r="B3" t="s">
         <v>702</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" t="s">
         <v>716</v>
       </c>
     </row>
@@ -14749,7 +15713,7 @@
       <c r="B4" t="s">
         <v>702</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="47" t="s">
         <v>713</v>
       </c>
     </row>
@@ -14757,7 +15721,7 @@
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="45" t="s">
         <v>714</v>
       </c>
     </row>
@@ -14768,7 +15732,7 @@
       <c r="B6" t="s">
         <v>702</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="46" t="s">
         <v>717</v>
       </c>
     </row>
@@ -14776,7 +15740,7 @@
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="46" t="s">
         <v>718</v>
       </c>
     </row>
@@ -14784,7 +15748,7 @@
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="46" t="s">
         <v>729</v>
       </c>
     </row>
@@ -14792,7 +15756,7 @@
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="46" t="s">
         <v>733</v>
       </c>
     </row>
@@ -14803,7 +15767,7 @@
       <c r="B10" t="s">
         <v>702</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="46" t="s">
         <v>736</v>
       </c>
     </row>
@@ -14814,7 +15778,7 @@
       <c r="B11" t="s">
         <v>702</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" t="s">
         <v>719</v>
       </c>
     </row>
@@ -14822,7 +15786,7 @@
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="46" t="s">
         <v>720</v>
       </c>
     </row>
@@ -14830,7 +15794,7 @@
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="46" t="s">
         <v>727</v>
       </c>
     </row>
@@ -14838,7 +15802,7 @@
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="46" t="s">
         <v>724</v>
       </c>
     </row>
@@ -14849,7 +15813,7 @@
       <c r="B15" t="s">
         <v>702</v>
       </c>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="46" t="s">
         <v>725</v>
       </c>
     </row>
@@ -14857,7 +15821,7 @@
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="46" t="s">
         <v>726</v>
       </c>
     </row>
@@ -14868,7 +15832,7 @@
       <c r="B17" t="s">
         <v>702</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="46" t="s">
         <v>730</v>
       </c>
     </row>
@@ -14879,7 +15843,7 @@
       <c r="B18" t="s">
         <v>702</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="46" t="s">
         <v>731</v>
       </c>
     </row>
@@ -14893,7 +15857,7 @@
       <c r="B20" t="s">
         <v>702</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="46" t="s">
         <v>732</v>
       </c>
     </row>
@@ -14907,7 +15871,7 @@
       <c r="B22" t="s">
         <v>702</v>
       </c>
-      <c r="C22" s="48" t="s">
+      <c r="C22" s="46" t="s">
         <v>739</v>
       </c>
     </row>
@@ -14918,7 +15882,7 @@
       <c r="B23" t="s">
         <v>702</v>
       </c>
-      <c r="C23" s="45" t="s">
+      <c r="C23" t="s">
         <v>930</v>
       </c>
     </row>
@@ -14929,7 +15893,7 @@
       <c r="B24" t="s">
         <v>702</v>
       </c>
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="46" t="s">
         <v>728</v>
       </c>
     </row>
@@ -14940,7 +15904,7 @@
       <c r="A26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="48" t="s">
+      <c r="C26" s="46" t="s">
         <v>721</v>
       </c>
     </row>
@@ -14951,7 +15915,7 @@
       <c r="B27" t="s">
         <v>702</v>
       </c>
-      <c r="C27" s="48" t="s">
+      <c r="C27" s="46" t="s">
         <v>722</v>
       </c>
     </row>
@@ -14959,7 +15923,7 @@
       <c r="A28" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="48" t="s">
+      <c r="C28" s="46" t="s">
         <v>737</v>
       </c>
     </row>
@@ -14970,7 +15934,7 @@
       <c r="B29" t="s">
         <v>702</v>
       </c>
-      <c r="C29" s="48" t="s">
+      <c r="C29" s="46" t="s">
         <v>738</v>
       </c>
     </row>
@@ -14981,7 +15945,7 @@
       <c r="B30" t="s">
         <v>702</v>
       </c>
-      <c r="C30" s="48" t="s">
+      <c r="C30" s="46" t="s">
         <v>734</v>
       </c>
     </row>
@@ -14989,7 +15953,7 @@
       <c r="A31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="48" t="s">
+      <c r="C31" s="46" t="s">
         <v>735</v>
       </c>
     </row>
@@ -15000,7 +15964,7 @@
       <c r="B32" t="s">
         <v>702</v>
       </c>
-      <c r="C32" s="48" t="s">
+      <c r="C32" s="46" t="s">
         <v>723</v>
       </c>
     </row>

</xml_diff>